<commit_message>
Change Sheet Page Name
</commit_message>
<xml_diff>
--- a/Documents/Philos FlashCards.xlsx
+++ b/Documents/Philos FlashCards.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/powerspots/GameStudio/WisdomSeekers/Mindscapes/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D668BA3C-3A93-F946-AF67-D501E739D0BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B32B6C7-C975-D944-BD34-A96B4A2EE412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Flash_Cards" sheetId="1" r:id="rId1"/>
+    <sheet name="FlashCards" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>

</xml_diff>